<commit_message>
added summary statistics to figure2, started with figure3
</commit_message>
<xml_diff>
--- a/fig2/Supplements2.xlsx
+++ b/fig2/Supplements2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTOF\MethodPaper\fig2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E113C-0865-4140-B72E-9F6C7B2C3C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3CD1FD-E358-43C3-B894-A9A7F40C1C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical_Standards" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,10 @@
     <sheet name="Literature_MassShifts_Database" sheetId="25" r:id="rId7"/>
     <sheet name="Sheet3" sheetId="9" r:id="rId8"/>
     <sheet name="G3P" sheetId="23" r:id="rId9"/>
-    <sheet name="DAP" sheetId="24" r:id="rId10"/>
-    <sheet name="Results_hmdb" sheetId="20" r:id="rId11"/>
-    <sheet name="Fraction_Groups" sheetId="21" r:id="rId12"/>
+    <sheet name="ADP" sheetId="24" r:id="rId10"/>
+    <sheet name="Dap" sheetId="27" r:id="rId11"/>
+    <sheet name="Results_hmdb" sheetId="20" r:id="rId12"/>
+    <sheet name="Fraction_Groups" sheetId="21" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6923" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6923" uniqueCount="2004">
   <si>
     <t>#</t>
   </si>
@@ -6045,6 +6046,18 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Amino Acid</t>
+  </si>
+  <si>
+    <t>Glycolysis/sugar-phosphates</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>TCA</t>
   </si>
 </sst>
 </file>
@@ -7369,8 +7382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V162"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K161"/>
+    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13998,42 +14011,37 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06A1883-067D-4CE8-827B-EDF5553D5120}">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>191.102</v>
+        <v>426.02179999999998</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>192.10499999999999</v>
+        <v>427.02510000000001</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>213.08500000000001</v>
+        <v>448.00380000000001</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>229.05799999999999</v>
+        <v>463.97829999999999</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>235.066</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>333.04300000000001</v>
+        <v>545.98</v>
       </c>
     </row>
   </sheetData>
@@ -14042,6 +14050,51 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CEEAA3-5558-43DF-BD85-994F4016A0DF}">
+  <dimension ref="A2:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>191.10220000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>192.10499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>235.06569999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>333.04320000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>213.08500000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>229.05770000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D2C999-E07A-4065-9835-70E4A7CDB622}">
   <dimension ref="A1:J384"/>
   <sheetViews>
@@ -26349,7 +26402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944F4D74-2A0E-4E32-B619-EBD62A68137F}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -26469,12 +26522,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F335CE5-98B2-4E70-9F20-A0A7ACB492F7}">
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="78.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26503,7 +26557,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26517,7 +26571,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26531,7 +26585,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -26545,7 +26599,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26559,7 +26613,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26573,7 +26627,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -26587,7 +26641,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -26601,7 +26655,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -26615,7 +26669,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -26629,7 +26683,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -26643,7 +26697,7 @@
         <v>68</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -26657,7 +26711,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -26671,7 +26725,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -26685,7 +26739,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -26699,7 +26753,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -26713,7 +26767,7 @@
         <v>93</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -26727,7 +26781,7 @@
         <v>98</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -26741,7 +26795,7 @@
         <v>103</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -26755,7 +26809,7 @@
         <v>108</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -26769,7 +26823,7 @@
         <v>113</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -26783,7 +26837,7 @@
         <v>118</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -26797,7 +26851,7 @@
         <v>123</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -26811,7 +26865,7 @@
         <v>128</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -26825,7 +26879,7 @@
         <v>133</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -27539,7 +27593,7 @@
         <v>412</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -27553,7 +27607,7 @@
         <v>417</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -27567,7 +27621,7 @@
         <v>422</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -27581,7 +27635,7 @@
         <v>427</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -27595,7 +27649,7 @@
         <v>432</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -27609,7 +27663,7 @@
         <v>438</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -27623,7 +27677,7 @@
         <v>444</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -27637,7 +27691,7 @@
         <v>449</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -27651,7 +27705,7 @@
         <v>454</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -27665,7 +27719,7 @@
         <v>459</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -27679,7 +27733,7 @@
         <v>464</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -27693,7 +27747,7 @@
         <v>469</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -27707,7 +27761,7 @@
         <v>475</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -27721,7 +27775,7 @@
         <v>480</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -27735,7 +27789,7 @@
         <v>485</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -27749,7 +27803,7 @@
         <v>490</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -27763,7 +27817,7 @@
         <v>495</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -27777,7 +27831,7 @@
         <v>499</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -27791,7 +27845,7 @@
         <v>504</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>814</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -27805,7 +27859,7 @@
         <v>509</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -27819,7 +27873,7 @@
         <v>514</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -27833,7 +27887,7 @@
         <v>520</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -27847,7 +27901,7 @@
         <v>525</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -27861,7 +27915,7 @@
         <v>530</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -27875,7 +27929,7 @@
         <v>536</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -27889,7 +27943,7 @@
         <v>542</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -27903,7 +27957,7 @@
         <v>548</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -27917,7 +27971,7 @@
         <v>554</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -27931,7 +27985,7 @@
         <v>560</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>814</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -28070,8 +28124,8 @@
       <c r="C114" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D114" s="9" t="s">
-        <v>816</v>
+      <c r="D114" s="5" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -28084,8 +28138,8 @@
       <c r="C115" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="D115" s="9" t="s">
-        <v>816</v>
+      <c r="D115" s="5" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -28169,7 +28223,7 @@
         <v>651</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>814</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -28253,7 +28307,7 @@
         <v>683</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>812</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed find- and check interferences..use only check_interferences..its up2date
</commit_message>
<xml_diff>
--- a/fig2/Supplements2.xlsx
+++ b/fig2/Supplements2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTOF\MethodPaper\fig2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E8447D-D7D6-4650-BD5F-24C74004BC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96409DD-1C50-4CB3-8C33-4DB38AA66A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical_Standards" sheetId="1" r:id="rId1"/>
@@ -7391,8 +7391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V162"/>
   <sheetViews>
-    <sheetView topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26456,11 +26456,11 @@
         <v>3793</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:G4" si="0">SUM(F2:F3)</f>
+        <f>SUM(F2:F3)</f>
         <v>6495</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>SUM(G2:G3)</f>
         <v>1073</v>
       </c>
       <c r="H4" t="s">
@@ -26491,8 +26491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA16DE0-2AC9-4A7F-A268-C81B2D22E1D0}">
   <dimension ref="A1:D961"/>
   <sheetViews>
-    <sheetView topLeftCell="A943" workbookViewId="0">
-      <selection sqref="A1:D961"/>
+    <sheetView topLeftCell="A928" workbookViewId="0">
+      <selection activeCell="D973" sqref="D973"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45825,8 +45825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BA6050-BD4A-4102-AD00-B4C433BE8607}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changed 17062022, added adducts_per_spike-in analysis for figure 2 and committed some other changes
</commit_message>
<xml_diff>
--- a/fig2/Supplements2.xlsx
+++ b/fig2/Supplements2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QTOF\MethodPaper\fig2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E0A6F-5B45-4692-8C55-AEC0845255D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72C6638-A10C-4004-82E4-C121C631499E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical_Standards" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6295" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6304" uniqueCount="2002">
   <si>
     <t>#</t>
   </si>
@@ -6048,6 +6048,12 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Glyoxylate</t>
+  </si>
+  <si>
+    <t>Putrescine</t>
   </si>
 </sst>
 </file>
@@ -7372,8 +7378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V162"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7382,6 +7388,7 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7454,6 +7461,9 @@
       <c r="K2" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N2" t="s">
+        <v>152</v>
+      </c>
       <c r="U2" s="2" t="s">
         <v>556</v>
       </c>
@@ -7495,6 +7505,9 @@
       <c r="K3" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="U3" s="3" t="s">
         <v>85</v>
       </c>
@@ -7536,6 +7549,9 @@
       <c r="K4" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N4" t="s">
+        <v>527</v>
+      </c>
       <c r="U4" s="3" t="s">
         <v>857</v>
       </c>
@@ -7577,6 +7593,9 @@
       <c r="K5" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N5" t="s">
+        <v>2000</v>
+      </c>
       <c r="U5" s="3" t="s">
         <v>440</v>
       </c>
@@ -7618,6 +7637,9 @@
       <c r="K6" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N6" t="s">
+        <v>2001</v>
+      </c>
       <c r="U6" s="3" t="s">
         <v>201</v>
       </c>
@@ -7659,6 +7681,9 @@
       <c r="K7" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N7" t="s">
+        <v>785</v>
+      </c>
       <c r="U7" s="3" t="s">
         <v>80</v>
       </c>
@@ -7700,6 +7725,9 @@
       <c r="K8" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N8" t="s">
+        <v>179</v>
+      </c>
       <c r="U8" s="3" t="s">
         <v>643</v>
       </c>
@@ -7741,6 +7769,9 @@
       <c r="K9" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="N9" t="s">
+        <v>367</v>
+      </c>
       <c r="U9" s="3" t="s">
         <v>675</v>
       </c>
@@ -7781,6 +7812,9 @@
       </c>
       <c r="K10" s="5" t="s">
         <v>812</v>
+      </c>
+      <c r="N10" t="s">
+        <v>420</v>
       </c>
       <c r="U10" s="3" t="s">
         <v>195</v>
@@ -14158,7 +14192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E521FFDB-54FC-4E5A-9FAE-3F88DF099870}">
   <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -44604,8 +44638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42568173-C28C-47DD-93D0-C54926A88FA6}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45726,8 +45760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BA6050-BD4A-4102-AD00-B4C433BE8607}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46320,8 +46354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA0183C-B974-4A73-9B9F-DA84F287E066}">
   <dimension ref="A1:C961"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A394" workbookViewId="0">
+      <selection activeCell="A413" sqref="A413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>